<commit_message>
Adding SpinTest and needed  supplementary changes
</commit_message>
<xml_diff>
--- a/to_distribute/DistanceTrials.xlsx
+++ b/to_distribute/DistanceTrials.xlsx
@@ -1,30 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GSTstudent2017\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davee\Arduino\GST_Arduino_Robotics\to_distribute\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9F75EF-C85D-4F4A-8A55-735A30A4F293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="11710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Distance" sheetId="1" r:id="rId1"/>
+    <sheet name="rotation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Run</t>
   </si>
@@ -40,13 +53,19 @@
   <si>
     <t>In/Pwr (Corrected)</t>
   </si>
+  <si>
+    <t>Rotations</t>
+  </si>
+  <si>
+    <t>Total Angle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -79,7 +98,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,7 +156,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -178,7 +196,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Distance!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -275,7 +293,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$31</c:f>
+              <c:f>Distance!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -374,7 +392,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$31</c:f>
+              <c:f>Distance!$C$2:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -403,6 +421,494 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C272-4FFE-9E2B-EEDD0271AC68}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="350860104"/>
+        <c:axId val="350865024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="350860104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="350865024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="350865024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="350860104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Angle vs. Power</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rotation!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Angle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29414566929133856"/>
+                  <c:y val="1.7680081656459609E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>rotation!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>rotation!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1835.9999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B12A-4DDF-A59B-3ACF36B3A722}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -626,7 +1132,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1159,8 +2221,57 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F04B206-4BE9-4969-9780-60E00D828B75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1439,20 +2550,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +2580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1489,7 +2600,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1497,7 +2608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1505,7 +2616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1513,7 +2624,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1521,7 +2632,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1532,7 +2643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1540,7 +2651,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1548,7 +2659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1556,7 +2667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1564,7 +2675,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1575,7 +2686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1583,7 +2694,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1591,7 +2702,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1599,7 +2710,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1607,7 +2718,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1618,7 +2729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1626,7 +2737,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1634,7 +2745,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1642,7 +2753,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1650,7 +2761,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1661,7 +2772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1669,7 +2780,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1677,7 +2788,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1685,7 +2796,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1693,7 +2804,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1704,7 +2815,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1712,7 +2823,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1720,7 +2831,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1728,7 +2839,338 @@
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD090A9-2F52-42F7-83E5-5B2FB9F69ED7}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>360*C2</f>
+        <v>360</v>
+      </c>
+      <c r="F2">
+        <f>SLOPE(D:D,B:B)</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="G2" s="1">
+        <f>SLOPE(D7:D31,B7:B31)</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D3:D27" si="0">360*C7</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>250</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>255</v>
+      </c>
+      <c r="C27">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1835.9999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
adding spin calibration code
</commit_message>
<xml_diff>
--- a/to_distribute/DistanceTrials.xlsx
+++ b/to_distribute/DistanceTrials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davee\Arduino\GST_Arduino_Robotics\to_distribute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF90BED-9CB5-4F30-802C-5F3B6FA8CFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFF7194-BF18-47E2-B3E6-5B4D2D53F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="11710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distance" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Run</t>
   </si>
@@ -48,22 +48,25 @@
     <t>Distance (inches)</t>
   </si>
   <si>
-    <t>In/Pwr</t>
-  </si>
-  <si>
-    <t>In/Pwr (Corrected)</t>
-  </si>
-  <si>
     <t>Neg. Rot</t>
-  </si>
-  <si>
-    <t>Neg. Angle</t>
   </si>
   <si>
     <t>Pos. Rot.</t>
   </si>
   <si>
-    <t>Pos.  Angle</t>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +84,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,14 +114,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,7 +663,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Angle vs. Power</a:t>
+              <a:t>Negative</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ngle vs. Power</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -690,17 +716,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>rotation!$F$1</c:f>
+              <c:f>rotation!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pos.  Angle</c:v>
+                  <c:v>Neg. Rot</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -751,8 +777,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.29414566929133856"/>
-                  <c:y val="1.7680081656459609E-4"/>
+                  <c:x val="-0.45481598133566636"/>
+                  <c:y val="0.12483328937949742"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -801,7 +827,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>50</c:v>
@@ -886,27 +912,63 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>rotation!$F$2:$F$31</c:f>
+              <c:f>rotation!$C$2:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>360</c:v>
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>720</c:v>
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1080</c:v>
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1440</c:v>
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1800</c:v>
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1835.9999999999998</c:v>
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>390</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,6 +977,516 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B12A-4DDF-A59B-3ACF36B3A722}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="350860104"/>
+        <c:axId val="350865024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="350860104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="350865024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="350865024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="350860104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Positive Angle vs. Power</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rotation!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pos. Rot.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.5309602571867867E-2"/>
+                  <c:y val="0.34526617187205666"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>rotation!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>rotation!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>390</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5419-4370-A8D0-1113E7F58B41}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1178,6 +1750,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1695,6 +2307,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2255,16 +3383,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>39687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2286,6 +3414,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{617AA737-88AA-4EAD-BBDC-B211540132A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2560,7 +3726,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E1" sqref="E1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2579,12 +3745,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -2596,14 +3756,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <f>SLOPE(C:C,B:B)</f>
-        <v>0.02</v>
-      </c>
-      <c r="F2" s="1">
-        <f>SLOPE(C7:C31,B7:B31)</f>
-        <v>0.02</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2861,19 +4014,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD090A9-2F52-42F7-83E5-5B2FB9F69ED7}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2881,25 +4034,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2907,78 +4048,98 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <f>360*C2</f>
-        <v>360</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <f>360*E2</f>
-        <v>360</v>
-      </c>
-      <c r="H2">
-        <f>SLOPE(F:F,B:B)</f>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="I2" s="1">
-        <f>SLOPE(F7:F31,B7:B31)</f>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
+      <c r="C3">
+        <v>60</v>
+      </c>
       <c r="D3">
-        <f t="shared" ref="D3:D31" si="0">360*C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>50</v>
       </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <f>SLOPE(C2:C31,$B2:$B31)</f>
+        <v>1.5993906154783666</v>
+      </c>
+      <c r="O5">
+        <f>SLOPE(D2:D31,$B2:$B31)</f>
+        <v>1.6018281535648993</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>AVERAGE(N5:O5)</f>
+        <v>1.6006093845216329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>50</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <f>INTERCEPT(C2:C31,$B2:$B31)</f>
+        <v>-19.286816981515273</v>
+      </c>
+      <c r="O6">
+        <f>INTERCEPT(D2:D31,$B2:$B31)</f>
+        <v>-19.695104611009498</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>AVERAGE(N6:O6)</f>
+        <v>-19.490960796262385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2986,69 +4147,57 @@
         <v>100</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>135</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>720</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F27" si="1">360*E7</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>100</v>
       </c>
+      <c r="C8">
+        <v>135</v>
+      </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
+      <c r="C9">
+        <v>135</v>
+      </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3056,69 +4205,59 @@
         <v>150</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <f>135+90</f>
+        <v>225</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1080</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <f>135+90</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>150</v>
       </c>
+      <c r="C13">
+        <v>225</v>
+      </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>150</v>
       </c>
+      <c r="C14">
+        <v>225</v>
+      </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>150</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>150</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3126,69 +4265,57 @@
         <v>200</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>315</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>1440</v>
-      </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>200</v>
       </c>
+      <c r="C18">
+        <v>310</v>
+      </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>200</v>
       </c>
+      <c r="C19">
+        <v>310</v>
+      </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>200</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>200</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3196,133 +4323,112 @@
         <v>250</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>365</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="E22">
-        <v>5</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>250</v>
       </c>
+      <c r="C23">
+        <v>370</v>
+      </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>250</v>
       </c>
+      <c r="C24">
+        <v>375</v>
+      </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>250</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>250</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>255</v>
       </c>
+      <c r="C27">
+        <v>390</v>
+      </c>
       <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
-        <v>1835.9999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>255</v>
       </c>
+      <c r="C28">
+        <v>390</v>
+      </c>
       <c r="D28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>255</v>
       </c>
+      <c r="C29">
+        <v>390</v>
+      </c>
       <c r="D29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>255</v>
       </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>255</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>